<commit_message>
found new receive code to get remote codes
</commit_message>
<xml_diff>
--- a/Arduino/remote codes.xlsx
+++ b/Arduino/remote codes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leefer_feefer/Desktop/Apps/Bluetooth Practice/Arduino/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leefer_feefer/Desktop/Apps/Ultra Universal Remote/Arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -84,8 +84,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -94,11 +96,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -386,12 +390,12 @@
     <col min="6" max="6" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13232</v>
       </c>
@@ -412,8 +416,12 @@
         <f>"pulseIR(" &amp; C3 &amp; ");"</f>
         <v>pulseIR(9420);</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="str">
+        <f>","&amp;A3&amp;","&amp;C3</f>
+        <v>,13232,9420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4540</v>
       </c>
@@ -434,8 +442,12 @@
         <f t="shared" ref="F4:F40" si="1">"pulseIR(" &amp; C4 &amp; ");"</f>
         <v>pulseIR(640);</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H67" si="2">","&amp;A4&amp;","&amp;C4</f>
+        <v>,4540,640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>520</v>
       </c>
@@ -456,8 +468,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(640);</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>,520,640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1640</v>
       </c>
@@ -478,8 +494,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(640);</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>,1640,640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1640</v>
       </c>
@@ -500,8 +520,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(640);</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>,1640,640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1660</v>
       </c>
@@ -522,8 +546,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(640);</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>500</v>
       </c>
@@ -544,8 +572,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>,500,620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1680</v>
       </c>
@@ -566,8 +598,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1660</v>
       </c>
@@ -588,8 +624,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1660</v>
       </c>
@@ -610,8 +650,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1660</v>
       </c>
@@ -632,8 +676,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1680</v>
       </c>
@@ -654,8 +702,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1660</v>
       </c>
@@ -676,8 +728,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>540</v>
       </c>
@@ -698,8 +754,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>540</v>
       </c>
@@ -720,8 +780,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>540</v>
       </c>
@@ -742,8 +806,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>540</v>
       </c>
@@ -764,8 +832,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1680</v>
       </c>
@@ -786,8 +858,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1660</v>
       </c>
@@ -808,8 +884,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1660</v>
       </c>
@@ -830,8 +910,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1680</v>
       </c>
@@ -852,8 +936,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1680</v>
       </c>
@@ -874,8 +962,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1680</v>
       </c>
@@ -896,8 +988,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>540</v>
       </c>
@@ -918,8 +1014,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1660</v>
       </c>
@@ -940,8 +1040,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>540</v>
       </c>
@@ -962,8 +1066,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>520</v>
       </c>
@@ -984,8 +1092,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>,520,620</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1680</v>
       </c>
@@ -1006,8 +1118,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1680</v>
       </c>
@@ -1028,8 +1144,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>540</v>
       </c>
@@ -1050,8 +1170,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1660</v>
       </c>
@@ -1072,8 +1196,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>540</v>
       </c>
@@ -1094,8 +1222,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1660</v>
       </c>
@@ -1116,8 +1248,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1680</v>
       </c>
@@ -1138,8 +1274,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>34860</v>
       </c>
@@ -1160,8 +1300,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(9340);</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>,34860,9340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4560</v>
       </c>
@@ -1182,8 +1326,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(620);</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>,4560,620</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>540</v>
       </c>
@@ -1204,8 +1352,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1680</v>
       </c>
@@ -1226,8 +1378,12 @@
         <f t="shared" si="1"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1680</v>
       </c>
@@ -1241,15 +1397,19 @@
         <v>2</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" ref="E41:E70" si="2">"delayMicroseconds(" &amp; A41 &amp; ");"</f>
+        <f t="shared" ref="E41:E70" si="3">"delayMicroseconds(" &amp; A41 &amp; ");"</f>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" ref="F41:F70" si="3">"pulseIR(" &amp; C41 &amp; ");"</f>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F41:F70" si="4">"pulseIR(" &amp; C41 &amp; ");"</f>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1680</v>
       </c>
@@ -1263,15 +1423,19 @@
         <v>2</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,600</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>540</v>
       </c>
@@ -1285,15 +1449,19 @@
         <v>2</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1660</v>
       </c>
@@ -1307,15 +1475,19 @@
         <v>2</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1660);</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1680</v>
       </c>
@@ -1329,15 +1501,19 @@
         <v>2</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1660</v>
       </c>
@@ -1351,15 +1527,19 @@
         <v>2</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1660);</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1660</v>
       </c>
@@ -1373,15 +1553,19 @@
         <v>2</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1660);</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1680</v>
       </c>
@@ -1395,15 +1579,19 @@
         <v>2</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H48" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1680</v>
       </c>
@@ -1417,15 +1605,19 @@
         <v>2</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>520</v>
       </c>
@@ -1439,15 +1631,19 @@
         <v>2</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(520);</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="2"/>
+        <v>,520,620</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>540</v>
       </c>
@@ -1461,15 +1657,19 @@
         <v>2</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>540</v>
       </c>
@@ -1483,15 +1683,19 @@
         <v>2</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>520</v>
       </c>
@@ -1505,15 +1709,19 @@
         <v>2</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(520);</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="2"/>
+        <v>,520,620</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1680</v>
       </c>
@@ -1527,15 +1735,19 @@
         <v>2</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H54" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,600</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1680</v>
       </c>
@@ -1549,15 +1761,19 @@
         <v>2</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>540</v>
       </c>
@@ -1571,15 +1787,19 @@
         <v>2</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H56" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1680</v>
       </c>
@@ -1593,15 +1813,19 @@
         <v>2</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>520</v>
       </c>
@@ -1615,15 +1839,19 @@
         <v>2</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(520);</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="2"/>
+        <v>,520,620</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>540</v>
       </c>
@@ -1637,15 +1865,19 @@
         <v>2</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>540</v>
       </c>
@@ -1659,15 +1891,19 @@
         <v>2</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>520</v>
       </c>
@@ -1681,15 +1917,19 @@
         <v>2</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(520);</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="2"/>
+        <v>,520,620</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>540</v>
       </c>
@@ -1703,15 +1943,19 @@
         <v>2</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>540</v>
       </c>
@@ -1725,15 +1969,19 @@
         <v>2</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>pulseIR(600);</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H63" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,600</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1680</v>
       </c>
@@ -1747,15 +1995,19 @@
         <v>2</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="2"/>
+        <v>,1680,620</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1660</v>
       </c>
@@ -1769,15 +2021,19 @@
         <v>2</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1660);</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>540</v>
       </c>
@@ -1791,15 +2047,19 @@
         <v>2</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="2"/>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1660</v>
       </c>
@@ -1813,15 +2073,19 @@
         <v>2</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1660);</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="2"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>540</v>
       </c>
@@ -1835,15 +2099,19 @@
         <v>2</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(540);</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" ref="H68:H70" si="5">","&amp;A68&amp;","&amp;C68</f>
+        <v>,540,620</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1660</v>
       </c>
@@ -1857,15 +2125,19 @@
         <v>2</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1660);</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="5"/>
+        <v>,1660,620</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1680</v>
       </c>
@@ -1879,12 +2151,16 @@
         <v>2</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>delayMicroseconds(1680);</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="3"/>
-        <v>pulseIR(620);</v>
+        <f t="shared" si="4"/>
+        <v>pulseIR(620);</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="5"/>
+        <v>,1680,620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>